<commit_message>
Age distribution csv file
used to get starting mean age. Calculated using birth rate and Census population age distribution for women
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuc43/Documents/GitHub/Weight-Loss-Medication-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/chen_liu_vanderbilt_edu/Documents/Decision Analysis 2/FINAL PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EC661D-D736-3742-995C-237AF5A0C611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1928" documentId="8_{6E917B29-0005-A044-87D0-797C44874429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1685AF57-DB06-494D-8551-092123808F12}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{96DC594E-6D50-554A-B2BF-BCE2D1A92884}"/>
+    <workbookView xWindow="-4380" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{96DC594E-6D50-554A-B2BF-BCE2D1A92884}"/>
   </bookViews>
   <sheets>
     <sheet name="Tradeoffs" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="305">
   <si>
     <t>p_healthy</t>
   </si>
@@ -958,7 +958,13 @@
     <t>Cost Input</t>
   </si>
   <si>
-    <t>fks;fkjas;dlkfjasl/dkfjl;askjfsd</t>
+    <t>Tirzapetide</t>
+  </si>
+  <si>
+    <t>Metformin</t>
+  </si>
+  <si>
+    <t>Xenical, Alli</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1163,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1358,6 +1364,18 @@
       </extLst>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3848,6 +3866,10 @@
 </FeaturePropertyBags>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4165,13 +4187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA39AF6A-B798-6841-9079-FBF9B902FB7B}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="185" zoomScaleNormal="190" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4322,20 +4344,56 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="81" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="81"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="81"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="81" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" s="81"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="81"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="81" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="81"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="29"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="B9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B10" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="https://icer.org/wp-content/uploads/2022/03/ICER_Obesity_Final_Evidence_Report_and_Meeting_Summary_102022.pdf" xr:uid="{8B0B475C-1445-0A49-8052-8B8940A26282}"/>
+    <hyperlink ref="A10" r:id="rId1" display="https://icer.org/wp-content/uploads/2022/03/ICER_Obesity_Final_Evidence_Report_and_Meeting_Summary_102022.pdf" xr:uid="{8B0B475C-1445-0A49-8052-8B8940A26282}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4345,7 +4403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA08B61-6711-E842-AE44-025E593BC187}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -4812,8 +4870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD35952-AB92-E844-A8E7-2CB3D4570E4F}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="131" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView zoomScale="160" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5395,10 +5453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466E40EB-D50E-2548-9AA6-8627F387D3D8}">
-  <dimension ref="A2:H104"/>
+  <dimension ref="A2:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6016,11 +6074,6 @@
       <c r="G97" s="38">
         <f>'CEA result 2yr pp'!D35</f>
         <v>-70</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -7199,8 +7252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D46EC1-E649-AE41-B9C7-6CC3E25C1038}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7368,12 +7421,10 @@
       <c r="B16" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>108</v>
-      </c>
+      <c r="C16" s="15">
+        <v>0</v>
+      </c>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -7767,10 +7818,9 @@
     <hyperlink ref="D12" r:id="rId1" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{5FAAD6D3-F882-3646-B222-CBC8C9ECE2E6}"/>
     <hyperlink ref="D13" r:id="rId2" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{DDFA0CAA-8BB1-F149-A546-0D05C86E9179}"/>
     <hyperlink ref="D14" r:id="rId3" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{DB8A4F04-F20A-1C40-8B92-72EE046C654C}"/>
-    <hyperlink ref="D16" r:id="rId4" display="https://doi-org.proxy.library.vanderbilt.edu/10.1111/cob.12294" xr:uid="{C2062E08-B4CE-AA4D-98D6-FB2026B2878A}"/>
-    <hyperlink ref="D48" r:id="rId5" display="https://www-ahajournals-org.proxy.library.vanderbilt.edu/doi/abs/10.1161/CIR.0000000000001258" xr:uid="{47710971-4F83-D44E-B505-73E64149644C}"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{F747604D-6A26-D840-A932-07D14ABE05A6}"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{2E72B5BD-456E-E140-B905-EFBC1801D5D9}"/>
+    <hyperlink ref="D48" r:id="rId4" display="https://www-ahajournals-org.proxy.library.vanderbilt.edu/doi/abs/10.1161/CIR.0000000000001258" xr:uid="{47710971-4F83-D44E-B505-73E64149644C}"/>
+    <hyperlink ref="D9" r:id="rId5" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{F747604D-6A26-D840-A932-07D14ABE05A6}"/>
+    <hyperlink ref="D10" r:id="rId6" display="https://doi.org/10.1161/CIR.0000000000001303" xr:uid="{2E72B5BD-456E-E140-B905-EFBC1801D5D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8428,7 +8478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FCA600-DA3A-374E-A964-F9CBC0FB34FF}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>

</xml_diff>